<commit_message>
Change C25 to 100pF to reduce high frequency attenuation
</commit_message>
<xml_diff>
--- a/amproc/BoM am na.xlsx
+++ b/amproc/BoM am na.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tom\Documents\Electronics\amtx\Audio\amproc\amproc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA659A1-D065-4E86-B767-1D7544E838D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E69685-4EF1-41AE-9CBA-74EE4F5B829C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="7275" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="amproc" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="284">
   <si>
     <t>Reference</t>
   </si>
   <si>
-    <t xml:space="preserve">C1 </t>
-  </si>
-  <si>
     <t>100p</t>
   </si>
   <si>
@@ -46,12 +43,6 @@
     <t>150n</t>
   </si>
   <si>
-    <t xml:space="preserve">C25 </t>
-  </si>
-  <si>
-    <t>560p</t>
-  </si>
-  <si>
     <t xml:space="preserve">C26 C29 C16 C15 C9 C30 </t>
   </si>
   <si>
@@ -328,15 +319,6 @@
     <t>2763215</t>
   </si>
   <si>
-    <t>560pF 50V 5% C0G</t>
-  </si>
-  <si>
-    <t>K561J15C0GF5TL2</t>
-  </si>
-  <si>
-    <t>2860139</t>
-  </si>
-  <si>
     <t>T1-3/4</t>
   </si>
   <si>
@@ -887,6 +869,9 @@
   </si>
   <si>
     <t>1516277</t>
+  </si>
+  <si>
+    <t>C1 C25</t>
   </si>
 </sst>
 </file>
@@ -1748,11 +1733,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1772,63 +1755,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I2" s="7">
         <v>2860078</v>
@@ -1838,72 +1821,72 @@
       </c>
       <c r="K2" s="8">
         <f>B2*J2</f>
-        <v>7.1300000000000002E-2</v>
+        <v>0.1426</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>245</v>
-      </c>
-      <c r="D3" t="s">
-        <v>277</v>
-      </c>
-      <c r="E3" t="s">
-        <v>249</v>
-      </c>
-      <c r="F3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" t="s">
-        <v>250</v>
-      </c>
-      <c r="H3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>251</v>
       </c>
       <c r="J3" s="8">
         <v>0.55500000000000005</v>
       </c>
       <c r="K3" s="8">
-        <f t="shared" ref="K3:K51" si="0">B3*J3</f>
+        <f t="shared" ref="K3:K50" si="0">B3*J3</f>
         <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="J4" s="8">
         <v>0.115</v>
@@ -1915,31 +1898,31 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="F5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="J5" s="8">
         <v>0.439</v>
@@ -1951,31 +1934,31 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J6" s="8">
         <v>8.2299999999999998E-2</v>
@@ -1987,31 +1970,31 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J7" s="8">
         <v>0.128</v>
@@ -2023,31 +2006,31 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J8" s="8">
         <v>0.13700000000000001</v>
@@ -2059,335 +2042,338 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="J9" s="8">
-        <v>0.13500000000000001</v>
+        <v>7.4499999999999997E-2</v>
       </c>
       <c r="K9" s="8">
         <f t="shared" si="0"/>
-        <v>0.13500000000000001</v>
+        <v>0.44699999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D10" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J10" s="8">
-        <v>7.4499999999999997E-2</v>
+        <v>0.13</v>
       </c>
       <c r="K10" s="8">
         <f t="shared" si="0"/>
-        <v>0.44699999999999995</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>230</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>238</v>
       </c>
       <c r="D11" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>249</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G11" t="s">
-        <v>97</v>
+        <v>250</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="J11" s="8">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="K11" s="8">
         <f t="shared" si="0"/>
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>244</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E12" t="s">
-        <v>255</v>
+        <v>96</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G12" t="s">
-        <v>256</v>
+        <v>97</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>257</v>
+        <v>98</v>
       </c>
       <c r="J12" s="8">
-        <v>0.11</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="K12" s="8">
         <f t="shared" si="0"/>
-        <v>0.11</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D13" t="s">
-        <v>279</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="G13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J13" s="8">
-        <v>0.27500000000000002</v>
+        <v>6.0900000000000003E-2</v>
       </c>
       <c r="K13" s="8">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>6.0900000000000003E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" t="s">
         <v>105</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" t="s">
         <v>106</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="G14" t="s">
-        <v>108</v>
-      </c>
-      <c r="H14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="J14" s="8">
-        <v>6.0900000000000003E-2</v>
+        <v>3.1899999999999998E-2</v>
       </c>
       <c r="K14" s="8">
         <f t="shared" si="0"/>
-        <v>6.0900000000000003E-2</v>
+        <v>0.19139999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
         <v>110</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>111</v>
       </c>
-      <c r="F15" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H15" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>113</v>
-      </c>
       <c r="J15" s="8">
-        <v>3.1899999999999998E-2</v>
+        <v>0.193</v>
       </c>
       <c r="K15" s="8">
         <f t="shared" si="0"/>
-        <v>0.19139999999999999</v>
+        <v>1.1579999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C16" s="2"/>
       <c r="D16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I16" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="G16" t="s">
-        <v>117</v>
-      </c>
-      <c r="H16" t="s">
-        <v>79</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>118</v>
-      </c>
       <c r="J16" s="8">
-        <v>0.193</v>
+        <v>0.59</v>
       </c>
       <c r="K16" s="8">
         <f t="shared" si="0"/>
-        <v>1.1579999999999999</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" t="s">
+        <v>118</v>
+      </c>
+      <c r="H17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="K17" s="8">
+        <f t="shared" si="0"/>
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="L17" t="s">
         <v>123</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="J17" s="8">
-        <v>0.59</v>
-      </c>
-      <c r="K17" s="8">
-        <f t="shared" si="0"/>
-        <v>1.77</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>124</v>
@@ -2399,1229 +2385,1190 @@
         <v>126</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J18" s="8">
-        <v>0.58099999999999996</v>
+        <v>0.247</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="0"/>
-        <v>0.58099999999999996</v>
+        <v>0.247</v>
       </c>
       <c r="L18" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" t="s">
         <v>130</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" t="s">
         <v>131</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="G19" t="s">
-        <v>133</v>
-      </c>
-      <c r="H19" t="s">
-        <v>79</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>134</v>
-      </c>
       <c r="J19" s="8">
-        <v>0.247</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="0"/>
-        <v>0.247</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="L19" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" t="s">
         <v>135</v>
       </c>
-      <c r="E20" t="s">
-        <v>136</v>
-      </c>
-      <c r="F20" t="s">
-        <v>132</v>
-      </c>
-      <c r="G20" t="s">
-        <v>137</v>
-      </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>138</v>
       </c>
       <c r="J20" s="8">
-        <v>0.13200000000000001</v>
+        <v>2.52E-2</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="0"/>
-        <v>0.13200000000000001</v>
+        <v>2.52E-2</v>
       </c>
       <c r="L20" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>277</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>278</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
+        <v>279</v>
       </c>
       <c r="E21" t="s">
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="F21" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G21" t="s">
-        <v>141</v>
+        <v>281</v>
       </c>
       <c r="H21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>144</v>
+        <v>282</v>
       </c>
       <c r="J21" s="8">
-        <v>2.52E-2</v>
+        <v>9.2499999999999999E-2</v>
       </c>
       <c r="K21" s="8">
         <f t="shared" si="0"/>
-        <v>2.52E-2</v>
-      </c>
-      <c r="L21" t="s">
-        <v>145</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>283</v>
+        <v>27</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>284</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>285</v>
+        <v>140</v>
       </c>
       <c r="E22" t="s">
-        <v>286</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="G22" t="s">
-        <v>287</v>
+        <v>142</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>288</v>
+        <v>144</v>
       </c>
       <c r="J22" s="8">
-        <v>9.2499999999999999E-2</v>
+        <v>0.151</v>
       </c>
       <c r="K22" s="8">
         <f t="shared" si="0"/>
-        <v>0.185</v>
+        <v>0.45299999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F23" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" t="s">
+        <v>143</v>
+      </c>
+      <c r="H23" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F23" t="s">
-        <v>116</v>
-      </c>
-      <c r="G23" t="s">
-        <v>148</v>
-      </c>
-      <c r="H23" t="s">
-        <v>79</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>150</v>
-      </c>
       <c r="J23" s="8">
-        <v>0.151</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="K23" s="8">
         <f t="shared" si="0"/>
-        <v>0.45299999999999996</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24">
-        <v>6</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>33</v>
+        <v>2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F24" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="G24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J24" s="8">
-        <v>0.16400000000000001</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="K24" s="8">
         <f t="shared" si="0"/>
-        <v>0.98399999999999999</v>
+        <v>5.7599999999999998E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>227</v>
       </c>
       <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" s="2">
-        <v>56</v>
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>242</v>
       </c>
       <c r="D25" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E25" t="s">
-        <v>158</v>
+        <v>252</v>
       </c>
       <c r="F25" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G25" t="s">
-        <v>154</v>
+        <v>254</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>156</v>
+        <v>255</v>
       </c>
       <c r="J25" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="0"/>
-        <v>5.7599999999999998E-2</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>233</v>
+        <v>32</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>248</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" t="s">
         <v>153</v>
       </c>
-      <c r="E26" t="s">
-        <v>258</v>
-      </c>
-      <c r="F26" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" t="s">
-        <v>260</v>
-      </c>
       <c r="H26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>261</v>
+        <v>154</v>
       </c>
       <c r="J26" s="8">
-        <v>2.8799999999999999E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>5.6800000000000003E-2</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D27" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F27" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G27" t="s">
         <v>159</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="J27" s="8">
-        <v>2.8400000000000002E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="0"/>
-        <v>5.6800000000000003E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>229</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>240</v>
       </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E28" t="s">
-        <v>161</v>
+        <v>256</v>
       </c>
       <c r="F28" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G28" t="s">
-        <v>165</v>
+        <v>257</v>
       </c>
       <c r="H28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>170</v>
+        <v>266</v>
       </c>
       <c r="J28" s="8">
-        <v>0.03</v>
+        <v>3.0200000000000001E-2</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.0200000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E29" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="F29" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G29" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="J29" s="8">
-        <v>3.0200000000000001E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K29" s="8">
         <f t="shared" si="0"/>
-        <v>3.0200000000000001E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>234</v>
+        <v>36</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>247</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E30" t="s">
-        <v>259</v>
+        <v>156</v>
       </c>
       <c r="F30" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G30" t="s">
-        <v>264</v>
+        <v>165</v>
       </c>
       <c r="H30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>265</v>
+        <v>166</v>
       </c>
       <c r="J30" s="8">
-        <v>2.8400000000000002E-2</v>
+        <v>2.86E-2</v>
       </c>
       <c r="K30" s="8">
         <f t="shared" si="0"/>
-        <v>2.8400000000000002E-2</v>
+        <v>2.86E-2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E31" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F31" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G31" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="H31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="J31" s="8">
-        <v>2.86E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K31" s="8">
         <f t="shared" si="0"/>
-        <v>2.86E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E32" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G32" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J32" s="8">
-        <v>0.03</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="K32" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>236</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>44</v>
+        <v>232</v>
       </c>
       <c r="D33" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
-        <v>174</v>
+        <v>260</v>
       </c>
       <c r="F33" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G33" t="s">
-        <v>175</v>
+        <v>261</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>176</v>
+        <v>262</v>
       </c>
       <c r="J33" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="K33" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>5.7599999999999998E-2</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D34" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F34" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G34" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="J34" s="8">
-        <v>2.8799999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K34" s="8">
         <f t="shared" si="0"/>
-        <v>5.7599999999999998E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>243</v>
+        <v>174</v>
       </c>
       <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>239</v>
+        <v>5</v>
+      </c>
+      <c r="C35" s="2">
+        <v>100</v>
       </c>
       <c r="D35" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E35" t="s">
-        <v>269</v>
+        <v>171</v>
       </c>
       <c r="F35" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G35" t="s">
-        <v>270</v>
+        <v>172</v>
       </c>
       <c r="H35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>271</v>
+        <v>173</v>
       </c>
       <c r="J35" s="8">
         <v>0.03</v>
       </c>
       <c r="K35" s="8">
         <f t="shared" si="0"/>
-        <v>0.06</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>42</v>
       </c>
       <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="F36" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G36" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="H36" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J36" s="8">
-        <v>0.03</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="K36" s="8">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="C37" s="2">
+        <v>470</v>
       </c>
       <c r="D37" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E37" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="F37" t="s">
-        <v>107</v>
+        <v>180</v>
       </c>
       <c r="G37" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="H37" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>182</v>
       </c>
       <c r="J37" s="8">
-        <v>2.8799999999999999E-2</v>
+        <v>7.8600000000000003E-2</v>
       </c>
       <c r="K37" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>0.15720000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38" s="2">
-        <v>470</v>
+        <v>4</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E38" t="s">
         <v>183</v>
       </c>
       <c r="F38" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" t="s">
+        <v>162</v>
+      </c>
+      <c r="H38" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="G38" t="s">
-        <v>187</v>
-      </c>
-      <c r="H38" t="s">
-        <v>79</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="J38" s="8">
-        <v>7.8600000000000003E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K38" s="8">
         <f t="shared" si="0"/>
-        <v>0.15720000000000001</v>
+        <v>0.11360000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="D39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E39" t="s">
+        <v>187</v>
+      </c>
+      <c r="F39" t="s">
+        <v>101</v>
+      </c>
+      <c r="G39" t="s">
+        <v>188</v>
+      </c>
+      <c r="H39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="F39" t="s">
-        <v>107</v>
-      </c>
-      <c r="G39" t="s">
-        <v>168</v>
-      </c>
-      <c r="H39" t="s">
-        <v>79</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>192</v>
-      </c>
       <c r="J39" s="8">
-        <v>2.8400000000000002E-2</v>
+        <v>2.8299999999999999E-2</v>
       </c>
       <c r="K39" s="8">
         <f t="shared" si="0"/>
-        <v>0.11360000000000001</v>
+        <v>0.14149999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E40" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F40" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G40" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J40" s="8">
-        <v>2.8299999999999999E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K40" s="8">
         <f t="shared" si="0"/>
-        <v>0.14149999999999999</v>
+        <v>0.11360000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41">
-        <v>4</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>53</v>
+        <v>1</v>
+      </c>
+      <c r="C41" s="2">
+        <v>560</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E41" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="F41" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G41" t="s">
+        <v>192</v>
+      </c>
+      <c r="H41" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="H41" t="s">
-        <v>79</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>197</v>
-      </c>
       <c r="J41" s="8">
-        <v>2.8400000000000002E-2</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="K41" s="8">
         <f t="shared" si="0"/>
-        <v>0.11360000000000001</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>194</v>
       </c>
       <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2">
-        <v>560</v>
+        <v>11</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E42" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F42" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G42" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="H42" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="J42" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="K42" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>0.31679999999999997</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>200</v>
+        <v>53</v>
       </c>
       <c r="B43">
-        <v>11</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>55</v>
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E43" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F43" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G43" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="H43" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>201</v>
+        <v>267</v>
       </c>
       <c r="J43" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="K43" s="8">
         <f t="shared" si="0"/>
-        <v>0.31679999999999997</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" s="2">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="E44" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="F44" t="s">
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="G44" t="s">
-        <v>155</v>
+        <v>202</v>
       </c>
       <c r="H44" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>273</v>
+        <v>203</v>
       </c>
       <c r="J44" s="8">
-        <v>2.8799999999999999E-2</v>
+        <v>1.5</v>
       </c>
       <c r="K44" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>175</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>203</v>
+      <c r="C45" s="2">
+        <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E45" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F45" t="s">
-        <v>207</v>
+        <v>74</v>
       </c>
       <c r="G45" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H45" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J45" s="8">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="K45" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="B46">
-        <v>2</v>
-      </c>
-      <c r="C46" s="2">
-        <v>100</v>
+        <v>3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="E46" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="F46" t="s">
-        <v>77</v>
+        <v>201</v>
       </c>
       <c r="G46" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="H46" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="J46" s="8">
-        <v>1.4</v>
+        <v>1.25</v>
       </c>
       <c r="K46" s="8">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>199</v>
+        <v>56</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="E47" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F47" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="G47" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="H47" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="J47" s="8">
-        <v>1.25</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="K47" s="8">
         <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>5.43</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B48">
-        <v>6</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D48" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" t="s">
         <v>217</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
+        <v>213</v>
+      </c>
+      <c r="G48" t="s">
         <v>218</v>
       </c>
-      <c r="F48" t="s">
+      <c r="H48" t="s">
+        <v>76</v>
+      </c>
+      <c r="I48" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="G48" t="s">
-        <v>220</v>
-      </c>
-      <c r="H48" t="s">
-        <v>79</v>
-      </c>
-      <c r="I48" s="7" t="s">
-        <v>221</v>
-      </c>
       <c r="J48" s="8">
-        <v>0.90500000000000003</v>
+        <v>1.84</v>
       </c>
       <c r="K48" s="8">
         <f t="shared" si="0"/>
-        <v>5.43</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" t="s">
+        <v>220</v>
+      </c>
+      <c r="E49" t="s">
+        <v>221</v>
+      </c>
+      <c r="F49" t="s">
+        <v>110</v>
+      </c>
+      <c r="G49" t="s">
         <v>222</v>
       </c>
-      <c r="E49" t="s">
+      <c r="H49" t="s">
+        <v>76</v>
+      </c>
+      <c r="I49" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="F49" t="s">
-        <v>219</v>
-      </c>
-      <c r="G49" t="s">
-        <v>224</v>
-      </c>
-      <c r="H49" t="s">
-        <v>79</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="J49" s="8">
-        <v>1.84</v>
+        <v>0.46</v>
       </c>
       <c r="K49" s="8">
         <f t="shared" si="0"/>
-        <v>1.84</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D50" t="s">
+        <v>220</v>
+      </c>
+      <c r="E50" t="s">
+        <v>224</v>
+      </c>
+      <c r="F50" t="s">
+        <v>110</v>
+      </c>
+      <c r="G50" t="s">
+        <v>225</v>
+      </c>
+      <c r="H50" t="s">
+        <v>115</v>
+      </c>
+      <c r="I50" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E50" t="s">
-        <v>227</v>
-      </c>
-      <c r="F50" t="s">
-        <v>116</v>
-      </c>
-      <c r="G50" t="s">
-        <v>228</v>
-      </c>
-      <c r="H50" t="s">
-        <v>79</v>
-      </c>
-      <c r="I50" s="7" t="s">
-        <v>229</v>
-      </c>
       <c r="J50" s="8">
-        <v>0.46</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="K50" s="8">
         <f t="shared" si="0"/>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>65</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D51" t="s">
-        <v>226</v>
-      </c>
-      <c r="E51" t="s">
-        <v>230</v>
-      </c>
-      <c r="F51" t="s">
-        <v>116</v>
-      </c>
-      <c r="G51" t="s">
-        <v>231</v>
-      </c>
-      <c r="H51" t="s">
-        <v>121</v>
-      </c>
-      <c r="I51" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="J51" s="8">
         <v>0.40400000000000003</v>
       </c>
-      <c r="K51" s="8">
-        <f t="shared" si="0"/>
-        <v>0.40400000000000003</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J53" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="K53" s="4">
-        <f>SUM(K2:K51)</f>
-        <v>30.167800000000003</v>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J52" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K52" s="4">
+        <f>SUM(K2:K50)</f>
+        <v>30.104100000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed LPF, pre-emphasis component values in AM (NA and RoW) variants to correct bandwidth
</commit_message>
<xml_diff>
--- a/amproc/BoM am na.xlsx
+++ b/amproc/BoM am na.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tom\Documents\Electronics\amtx\Audio\amproc\amproc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E69685-4EF1-41AE-9CBA-74EE4F5B829C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A89BE8-59FD-4B45-95AA-563213D566AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7275" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="amproc" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="281">
   <si>
     <t>Reference</t>
   </si>
@@ -49,9 +49,6 @@
     <t>47u 25V</t>
   </si>
   <si>
-    <t xml:space="preserve">C4 </t>
-  </si>
-  <si>
     <t>1n</t>
   </si>
   <si>
@@ -715,21 +712,9 @@
     <t>C5</t>
   </si>
   <si>
-    <t>10n</t>
-  </si>
-  <si>
-    <t>18k</t>
-  </si>
-  <si>
-    <t>2k</t>
-  </si>
-  <si>
     <t>C10 C27</t>
   </si>
   <si>
-    <t>C11 C28</t>
-  </si>
-  <si>
     <t>R31 R45</t>
   </si>
   <si>
@@ -739,9 +724,6 @@
     <t>4n7</t>
   </si>
   <si>
-    <t>1n8</t>
-  </si>
-  <si>
     <t>3k9</t>
   </si>
   <si>
@@ -751,24 +733,6 @@
     <t>75k</t>
   </si>
   <si>
-    <t>1.8nF 100V 5% film</t>
-  </si>
-  <si>
-    <t>SMR5182J100J01L16.5CBULK</t>
-  </si>
-  <si>
-    <t>2529167</t>
-  </si>
-  <si>
-    <t>10nF 100V 5% film</t>
-  </si>
-  <si>
-    <t>R82EC2100CK50J</t>
-  </si>
-  <si>
-    <t>2710245</t>
-  </si>
-  <si>
     <t>4.7nF 100V 10% film</t>
   </si>
   <si>
@@ -802,24 +766,6 @@
     <t>2401783</t>
   </si>
   <si>
-    <t>18k 0.6W 1% metal film</t>
-  </si>
-  <si>
-    <t>MCMF006FF1802A50</t>
-  </si>
-  <si>
-    <t>2401787</t>
-  </si>
-  <si>
-    <t>2k 0.6W 1% metal film</t>
-  </si>
-  <si>
-    <t>MCMF006FF2001A50</t>
-  </si>
-  <si>
-    <t>2401761</t>
-  </si>
-  <si>
     <t>2401768</t>
   </si>
   <si>
@@ -872,6 +818,51 @@
   </si>
   <si>
     <t>C1 C25</t>
+  </si>
+  <si>
+    <t>24k</t>
+  </si>
+  <si>
+    <t>15k</t>
+  </si>
+  <si>
+    <t>470p</t>
+  </si>
+  <si>
+    <t>C4 C11 C28</t>
+  </si>
+  <si>
+    <t>Radial disc W4mm T2.5mm S5mm</t>
+  </si>
+  <si>
+    <t>470pF 60V 5% C0G</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>RDE5C1H471J0M1H03A</t>
+  </si>
+  <si>
+    <t>2990775</t>
+  </si>
+  <si>
+    <t>24k 0.6W 1% metal film</t>
+  </si>
+  <si>
+    <t>MCMF006FF2402A50</t>
+  </si>
+  <si>
+    <t>2401790</t>
+  </si>
+  <si>
+    <t>15k 0.6W 1% metal film</t>
+  </si>
+  <si>
+    <t>MCMF006FF1502A50</t>
+  </si>
+  <si>
+    <t>2401785</t>
   </si>
 </sst>
 </file>
@@ -1733,9 +1724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1755,42 +1748,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1799,19 +1792,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>74</v>
       </c>
-      <c r="G2" t="s">
-        <v>75</v>
-      </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I2" s="7">
         <v>2860078</v>
@@ -1826,579 +1819,582 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>239</v>
+        <v>268</v>
       </c>
       <c r="D3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" t="s">
         <v>271</v>
       </c>
-      <c r="E3" t="s">
-        <v>243</v>
-      </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>272</v>
       </c>
       <c r="G3" t="s">
-        <v>244</v>
+        <v>273</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>245</v>
+        <v>274</v>
       </c>
       <c r="J3" s="8">
-        <v>0.55500000000000005</v>
+        <v>0.16</v>
       </c>
       <c r="K3" s="8">
-        <f t="shared" ref="K3:K50" si="0">B3*J3</f>
-        <v>1.1100000000000001</v>
+        <f t="shared" ref="K3:K49" si="0">B3*J3</f>
+        <v>0.32</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>231</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="E4" t="s">
-        <v>246</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
         <v>81</v>
       </c>
-      <c r="G4" t="s">
-        <v>247</v>
-      </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>248</v>
+        <v>82</v>
       </c>
       <c r="J4" s="8">
-        <v>0.115</v>
+        <v>0.439</v>
       </c>
       <c r="K4" s="8">
         <f t="shared" si="0"/>
-        <v>0.23</v>
+        <v>0.878</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J5" s="8">
-        <v>0.439</v>
+        <v>8.2299999999999998E-2</v>
       </c>
       <c r="K5" s="8">
         <f t="shared" si="0"/>
-        <v>0.878</v>
+        <v>0.57609999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="J6" s="8">
-        <v>8.2299999999999998E-2</v>
+        <v>0.128</v>
       </c>
       <c r="K6" s="8">
         <f t="shared" si="0"/>
-        <v>0.57609999999999995</v>
+        <v>0.25600000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J7" s="8">
-        <v>0.128</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="K7" s="8">
         <f t="shared" si="0"/>
-        <v>0.25600000000000001</v>
+        <v>0.13700000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J8" s="8">
-        <v>0.13700000000000001</v>
+        <v>7.4499999999999997E-2</v>
       </c>
       <c r="K8" s="8">
         <f t="shared" si="0"/>
-        <v>0.13700000000000001</v>
+        <v>0.44699999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>269</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="J9" s="8">
-        <v>7.4499999999999997E-2</v>
+        <v>0.13</v>
       </c>
       <c r="K9" s="8">
         <f t="shared" si="0"/>
-        <v>0.44699999999999995</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>229</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>233</v>
       </c>
       <c r="D10" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>237</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>238</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>95</v>
+        <v>239</v>
       </c>
       <c r="J10" s="8">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="K10" s="8">
         <f t="shared" si="0"/>
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>238</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="E11" t="s">
-        <v>249</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>250</v>
+        <v>96</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>251</v>
+        <v>97</v>
       </c>
       <c r="J11" s="8">
-        <v>0.11</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="K11" s="8">
         <f t="shared" si="0"/>
-        <v>0.11</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>273</v>
+        <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="J12" s="8">
-        <v>0.27500000000000002</v>
+        <v>6.0900000000000003E-2</v>
       </c>
       <c r="K12" s="8">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>6.0900000000000003E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" t="s">
         <v>100</v>
       </c>
-      <c r="F13" t="s">
-        <v>101</v>
-      </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="J13" s="8">
-        <v>6.0900000000000003E-2</v>
+        <v>3.1899999999999998E-2</v>
       </c>
       <c r="K13" s="8">
         <f t="shared" si="0"/>
-        <v>6.0900000000000003E-2</v>
+        <v>0.19139999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G14" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="J14" s="8">
-        <v>3.1899999999999998E-2</v>
+        <v>0.193</v>
       </c>
       <c r="K14" s="8">
         <f t="shared" si="0"/>
-        <v>0.19139999999999999</v>
+        <v>1.1579999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C15" s="2"/>
       <c r="D15" t="s">
-        <v>108</v>
-      </c>
-      <c r="E15" t="s">
-        <v>109</v>
-      </c>
-      <c r="F15" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" t="s">
-        <v>111</v>
-      </c>
-      <c r="H15" t="s">
-        <v>76</v>
+        <v>112</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="J15" s="8">
-        <v>0.193</v>
+        <v>0.59</v>
       </c>
       <c r="K15" s="8">
         <f t="shared" si="0"/>
-        <v>1.1579999999999999</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
         <v>117</v>
       </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>115</v>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" t="s">
+        <v>75</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="J16" s="8">
-        <v>0.59</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="K16" s="8">
         <f t="shared" si="0"/>
-        <v>1.77</v>
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="L16" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F17" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="J17" s="8">
-        <v>0.58099999999999996</v>
+        <v>0.247</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="0"/>
-        <v>0.58099999999999996</v>
+        <v>0.247</v>
       </c>
       <c r="L17" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" t="s">
         <v>125</v>
       </c>
-      <c r="F18" t="s">
-        <v>126</v>
-      </c>
       <c r="G18" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="J18" s="8">
-        <v>0.247</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="0"/>
-        <v>0.247</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="L18" t="s">
         <v>136</v>
@@ -2406,656 +2402,653 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G19" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="J19" s="8">
-        <v>0.13200000000000001</v>
+        <v>2.52E-2</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="0"/>
-        <v>0.13200000000000001</v>
+        <v>2.52E-2</v>
       </c>
       <c r="L19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>260</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>261</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>262</v>
       </c>
       <c r="F20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G20" t="s">
-        <v>135</v>
+        <v>263</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>138</v>
+        <v>264</v>
       </c>
       <c r="J20" s="8">
-        <v>2.52E-2</v>
+        <v>9.2499999999999999E-2</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="0"/>
-        <v>2.52E-2</v>
-      </c>
-      <c r="L20" t="s">
-        <v>139</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>277</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>278</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>279</v>
+        <v>139</v>
       </c>
       <c r="E21" t="s">
-        <v>280</v>
+        <v>140</v>
       </c>
       <c r="F21" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
-        <v>281</v>
+        <v>141</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>282</v>
+        <v>143</v>
       </c>
       <c r="J21" s="8">
-        <v>9.2499999999999999E-2</v>
+        <v>0.151</v>
       </c>
       <c r="K21" s="8">
         <f t="shared" si="0"/>
-        <v>0.185</v>
+        <v>0.45299999999999996</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E22" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G22" t="s">
         <v>142</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J22" s="8">
-        <v>0.151</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="K22" s="8">
         <f t="shared" si="0"/>
-        <v>0.45299999999999996</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23">
-        <v>6</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F23" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J23" s="8">
-        <v>0.16400000000000001</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="K23" s="8">
         <f t="shared" si="0"/>
-        <v>0.98399999999999999</v>
+        <v>5.7599999999999998E-2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>226</v>
       </c>
       <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24" s="2">
-        <v>56</v>
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="D24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E24" t="s">
-        <v>152</v>
+        <v>240</v>
       </c>
       <c r="F24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>148</v>
+        <v>242</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>150</v>
+        <v>243</v>
       </c>
       <c r="J24" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="K24" s="8">
         <f t="shared" si="0"/>
-        <v>5.7599999999999998E-2</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>227</v>
+        <v>31</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>242</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E25" t="s">
-        <v>252</v>
+        <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>254</v>
+        <v>152</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>255</v>
+        <v>153</v>
       </c>
       <c r="J25" s="8">
-        <v>2.8799999999999999E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>5.6800000000000003E-2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E26" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G26" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="J26" s="8">
-        <v>2.8400000000000002E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="0"/>
-        <v>5.6800000000000003E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="D27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E27" t="s">
-        <v>155</v>
+        <v>244</v>
       </c>
       <c r="F27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>159</v>
+        <v>245</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>164</v>
+        <v>248</v>
       </c>
       <c r="J27" s="8">
-        <v>0.03</v>
+        <v>3.0200000000000001E-2</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>3.0200000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E28" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="F28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G28" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="H28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="J28" s="8">
-        <v>3.0200000000000001E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="0"/>
-        <v>3.0200000000000001E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>228</v>
+        <v>35</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>241</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E29" t="s">
-        <v>253</v>
+        <v>155</v>
       </c>
       <c r="F29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>258</v>
+        <v>164</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>259</v>
+        <v>165</v>
       </c>
       <c r="J29" s="8">
-        <v>2.8400000000000002E-2</v>
+        <v>2.86E-2</v>
       </c>
       <c r="K29" s="8">
         <f t="shared" si="0"/>
-        <v>2.8400000000000002E-2</v>
+        <v>2.86E-2</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E30" t="s">
         <v>156</v>
       </c>
       <c r="F30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G30" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>166</v>
       </c>
       <c r="J30" s="8">
-        <v>2.86E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K30" s="8">
         <f t="shared" si="0"/>
-        <v>2.86E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E31" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="F31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G31" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="H31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="J31" s="8">
-        <v>0.03</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="K31" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>231</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>41</v>
+        <v>266</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E32" t="s">
-        <v>168</v>
+        <v>275</v>
       </c>
       <c r="F32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G32" t="s">
-        <v>169</v>
+        <v>276</v>
       </c>
       <c r="H32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>170</v>
+        <v>277</v>
       </c>
       <c r="J32" s="8">
-        <v>2.8799999999999999E-2</v>
+        <v>3.7900000000000003E-2</v>
       </c>
       <c r="K32" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>7.5800000000000006E-2</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="D33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E33" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="F33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G33" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="H33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="J33" s="8">
-        <v>2.8799999999999999E-2</v>
+        <v>3.7900000000000003E-2</v>
       </c>
       <c r="K33" s="8">
         <f t="shared" si="0"/>
-        <v>5.7599999999999998E-2</v>
+        <v>7.5800000000000006E-2</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>237</v>
+        <v>173</v>
       </c>
       <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>233</v>
+        <v>5</v>
+      </c>
+      <c r="C34" s="2">
+        <v>100</v>
       </c>
       <c r="D34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E34" t="s">
-        <v>263</v>
+        <v>170</v>
       </c>
       <c r="F34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G34" t="s">
-        <v>264</v>
+        <v>171</v>
       </c>
       <c r="H34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>265</v>
+        <v>172</v>
       </c>
       <c r="J34" s="8">
         <v>0.03</v>
       </c>
       <c r="K34" s="8">
         <f t="shared" si="0"/>
-        <v>0.06</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="B35">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" t="s">
         <v>100</v>
       </c>
-      <c r="D35" t="s">
-        <v>147</v>
-      </c>
-      <c r="E35" t="s">
-        <v>171</v>
-      </c>
-      <c r="F35" t="s">
-        <v>101</v>
-      </c>
       <c r="G35" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="H35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J35" s="8">
-        <v>0.03</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="K35" s="8">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="C36" s="2">
+        <v>470</v>
       </c>
       <c r="D36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E36" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="F36" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="G36" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="H36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="J36" s="8">
-        <v>2.8799999999999999E-2</v>
+        <v>7.8600000000000003E-2</v>
       </c>
       <c r="K36" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>0.15720000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
@@ -3063,215 +3056,215 @@
         <v>44</v>
       </c>
       <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37" s="2">
-        <v>470</v>
+        <v>4</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E37" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="F37" t="s">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="G37" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="H37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="J37" s="8">
-        <v>7.8600000000000003E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K37" s="8">
         <f t="shared" si="0"/>
-        <v>0.15720000000000001</v>
+        <v>0.11360000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E38" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G38" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="H38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J38" s="8">
-        <v>2.8400000000000002E-2</v>
+        <v>2.8299999999999999E-2</v>
       </c>
       <c r="K38" s="8">
         <f t="shared" si="0"/>
-        <v>0.11360000000000001</v>
+        <v>0.14149999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E39" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G39" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J39" s="8">
-        <v>2.8299999999999999E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K39" s="8">
         <f t="shared" si="0"/>
-        <v>0.14149999999999999</v>
+        <v>0.11360000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B40">
-        <v>4</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>50</v>
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <v>560</v>
       </c>
       <c r="D40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E40" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G40" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="J40" s="8">
-        <v>2.8400000000000002E-2</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="K40" s="8">
         <f t="shared" si="0"/>
-        <v>0.11360000000000001</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41">
+        <v>11</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" s="2">
-        <v>560</v>
-      </c>
       <c r="D41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E41" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="F41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G41" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="H41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J41" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="K41" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>0.31679999999999997</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>52</v>
       </c>
       <c r="B42">
-        <v>11</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>52</v>
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E42" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G42" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="H42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>195</v>
+        <v>249</v>
       </c>
       <c r="J42" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="K42" s="8">
         <f t="shared" si="0"/>
-        <v>0.31679999999999997</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.4">
@@ -3279,296 +3272,260 @@
         <v>53</v>
       </c>
       <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="D43" t="s">
-        <v>147</v>
+        <v>197</v>
       </c>
       <c r="E43" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="F43" t="s">
-        <v>101</v>
+        <v>200</v>
       </c>
       <c r="G43" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="H43" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>267</v>
+        <v>202</v>
       </c>
       <c r="J43" s="8">
-        <v>2.8799999999999999E-2</v>
+        <v>1.5</v>
       </c>
       <c r="K43" s="8">
         <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>174</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>197</v>
+      <c r="C44" s="2">
+        <v>100</v>
       </c>
       <c r="D44" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="E44" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="F44" t="s">
-        <v>201</v>
+        <v>73</v>
       </c>
       <c r="G44" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="H44" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="J44" s="8">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="K44" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="B45">
-        <v>2</v>
-      </c>
-      <c r="C45" s="2">
-        <v>100</v>
+        <v>3</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D45" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E45" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F45" t="s">
-        <v>74</v>
+        <v>200</v>
       </c>
       <c r="G45" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H45" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="J45" s="8">
-        <v>1.4</v>
+        <v>1.25</v>
       </c>
       <c r="K45" s="8">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>193</v>
+        <v>55</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="E46" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="F46" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="G46" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="H46" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="J46" s="8">
-        <v>1.25</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="K46" s="8">
         <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>5.43</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E47" t="s">
+        <v>216</v>
+      </c>
+      <c r="F47" t="s">
         <v>212</v>
       </c>
-      <c r="F47" t="s">
-        <v>213</v>
-      </c>
       <c r="G47" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="J47" s="8">
-        <v>0.90500000000000003</v>
+        <v>1.84</v>
       </c>
       <c r="K47" s="8">
         <f t="shared" si="0"/>
-        <v>5.43</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D48" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E48" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F48" t="s">
-        <v>213</v>
+        <v>109</v>
       </c>
       <c r="G48" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="J48" s="8">
-        <v>1.84</v>
+        <v>0.46</v>
       </c>
       <c r="K48" s="8">
         <f t="shared" si="0"/>
-        <v>1.84</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E49" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G49" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="H49" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="J49" s="8">
-        <v>0.46</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="K49" s="8">
         <f t="shared" si="0"/>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" t="s">
-        <v>220</v>
-      </c>
-      <c r="E50" t="s">
-        <v>224</v>
-      </c>
-      <c r="F50" t="s">
-        <v>110</v>
-      </c>
-      <c r="G50" t="s">
-        <v>225</v>
-      </c>
-      <c r="H50" t="s">
-        <v>115</v>
-      </c>
-      <c r="I50" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="J50" s="8">
         <v>0.40400000000000003</v>
       </c>
-      <c r="K50" s="8">
-        <f t="shared" si="0"/>
-        <v>0.40400000000000003</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J52" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="K52" s="4">
-        <f>SUM(K2:K50)</f>
-        <v>30.104100000000003</v>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J51" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K51" s="4">
+        <f>SUM(K2:K49)</f>
+        <v>29.3781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change R10 to 430k to increase minimum release time
</commit_message>
<xml_diff>
--- a/amproc/BoM am na.xlsx
+++ b/amproc/BoM am na.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tom\Documents\Electronics\amtx\Audio\amproc\amproc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Electronics\amtx\Audio\amproc\amproc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A89BE8-59FD-4B45-95AA-563213D566AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102F5CB0-9700-4C80-B519-C354C7DDD0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="amproc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="286">
   <si>
     <t>Reference</t>
   </si>
@@ -166,9 +178,6 @@
     <t>2k2</t>
   </si>
   <si>
-    <t xml:space="preserve">R43 R29 R10 R1 </t>
-  </si>
-  <si>
     <t>100k</t>
   </si>
   <si>
@@ -863,6 +872,24 @@
   </si>
   <si>
     <t>2401785</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>430k</t>
+  </si>
+  <si>
+    <t>530k 0.6W 1% metal film</t>
+  </si>
+  <si>
+    <t>MCMF006FF4303A50</t>
+  </si>
+  <si>
+    <t>2401823</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R43 R29 R1 </t>
   </si>
 </sst>
 </file>
@@ -1724,66 +1751,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.61328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.4609375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23046875" style="4"/>
-    <col min="12" max="12" width="37.07421875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.28515625" style="4"/>
+    <col min="12" max="12" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1792,19 +1819,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
         <v>72</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>73</v>
       </c>
-      <c r="G2" t="s">
-        <v>74</v>
-      </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I2" s="7">
         <v>2860078</v>
@@ -1817,43 +1844,43 @@
         <v>0.1426</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E3" t="s">
         <v>270</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>271</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>272</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="H3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>274</v>
       </c>
       <c r="J3" s="8">
         <v>0.16</v>
       </c>
       <c r="K3" s="8">
-        <f t="shared" ref="K3:K49" si="0">B3*J3</f>
+        <f t="shared" ref="K3:K50" si="0">B3*J3</f>
         <v>0.32</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1864,22 +1891,22 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
         <v>79</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>80</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="J4" s="8">
         <v>0.439</v>
@@ -1889,9 +1916,9 @@
         <v>0.878</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -1900,22 +1927,22 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s">
         <v>76</v>
       </c>
-      <c r="F5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="H5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="J5" s="8">
         <v>8.2299999999999998E-2</v>
@@ -1925,9 +1952,9 @@
         <v>0.57609999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1936,22 +1963,22 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
         <v>86</v>
       </c>
-      <c r="F6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="H6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="J6" s="8">
         <v>0.128</v>
@@ -1961,7 +1988,7 @@
         <v>0.25600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1972,22 +1999,22 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" t="s">
         <v>89</v>
       </c>
-      <c r="F7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="H7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="J7" s="8">
         <v>0.13700000000000001</v>
@@ -1997,7 +2024,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2008,22 +2035,22 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
         <v>83</v>
       </c>
-      <c r="F8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H8" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="J8" s="8">
         <v>7.4499999999999997E-2</v>
@@ -2033,9 +2060,9 @@
         <v>0.44699999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2044,22 +2071,22 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
         <v>92</v>
       </c>
-      <c r="F9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="H9" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="J9" s="8">
         <v>0.13</v>
@@ -2069,33 +2096,33 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" t="s">
         <v>237</v>
       </c>
-      <c r="F10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="H10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="J10" s="8">
         <v>0.11</v>
@@ -2105,7 +2132,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2116,22 +2143,22 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" t="s">
         <v>95</v>
       </c>
-      <c r="F11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="H11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="J11" s="8">
         <v>0.27500000000000002</v>
@@ -2141,7 +2168,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2152,22 +2179,22 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" t="s">
         <v>98</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>99</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>100</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="J12" s="8">
         <v>6.0900000000000003E-2</v>
@@ -2177,7 +2204,7 @@
         <v>6.0900000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2188,22 +2215,22 @@
         <v>15</v>
       </c>
       <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" t="s">
         <v>103</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" t="s">
         <v>104</v>
       </c>
-      <c r="F13" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="H13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="J13" s="8">
         <v>3.1899999999999998E-2</v>
@@ -2213,7 +2240,7 @@
         <v>0.19139999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2224,22 +2251,22 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" t="s">
         <v>107</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>108</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>109</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="H14" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="J14" s="8">
         <v>0.193</v>
@@ -2249,31 +2276,31 @@
         <v>1.1579999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H15" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="J15" s="8">
         <v>0.59</v>
@@ -2283,7 +2310,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2294,22 +2321,22 @@
         <v>19</v>
       </c>
       <c r="D16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" t="s">
         <v>117</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>118</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="G16" t="s">
-        <v>117</v>
-      </c>
-      <c r="H16" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="J16" s="8">
         <v>0.58099999999999996</v>
@@ -2319,10 +2346,10 @@
         <v>0.58099999999999996</v>
       </c>
       <c r="L16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2333,22 +2360,22 @@
         <v>21</v>
       </c>
       <c r="D17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" t="s">
         <v>123</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>124</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>125</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="H17" t="s">
-        <v>75</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="J17" s="8">
         <v>0.247</v>
@@ -2358,10 +2385,10 @@
         <v>0.247</v>
       </c>
       <c r="L17" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2372,22 +2399,22 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" t="s">
         <v>128</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" t="s">
         <v>129</v>
       </c>
-      <c r="F18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="H18" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="J18" s="8">
         <v>0.13200000000000001</v>
@@ -2397,10 +2424,10 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="L18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2411,22 +2438,22 @@
         <v>25</v>
       </c>
       <c r="D19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" t="s">
         <v>132</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G19" t="s">
         <v>133</v>
       </c>
-      <c r="F19" t="s">
-        <v>125</v>
-      </c>
-      <c r="G19" t="s">
-        <v>134</v>
-      </c>
       <c r="H19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J19" s="8">
         <v>2.52E-2</v>
@@ -2436,36 +2463,36 @@
         <v>2.52E-2</v>
       </c>
       <c r="L19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" t="s">
         <v>260</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>261</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" t="s">
         <v>262</v>
       </c>
-      <c r="F20" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>263</v>
-      </c>
-      <c r="H20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>264</v>
       </c>
       <c r="J20" s="8">
         <v>9.2499999999999999E-2</v>
@@ -2475,7 +2502,7 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2486,22 +2513,22 @@
         <v>27</v>
       </c>
       <c r="D21" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" t="s">
         <v>139</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" t="s">
         <v>140</v>
       </c>
-      <c r="F21" t="s">
-        <v>109</v>
-      </c>
-      <c r="G21" t="s">
-        <v>141</v>
-      </c>
       <c r="H21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J21" s="8">
         <v>0.151</v>
@@ -2511,7 +2538,7 @@
         <v>0.45299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -2522,22 +2549,22 @@
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="F22" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" t="s">
-        <v>142</v>
-      </c>
-      <c r="H22" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="J22" s="8">
         <v>0.16400000000000001</v>
@@ -2547,187 +2574,186 @@
         <v>0.98399999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>280</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" t="s">
+        <v>282</v>
+      </c>
+      <c r="F23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" t="s">
+        <v>283</v>
+      </c>
+      <c r="H23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J23" s="8">
+        <v>2.07E-2</v>
+      </c>
+      <c r="K23" s="8">
+        <v>2.07E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>30</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>2</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C24" s="2">
         <v>56</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" t="s">
         <v>146</v>
       </c>
-      <c r="E23" t="s">
-        <v>151</v>
-      </c>
-      <c r="F23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" t="s">
-        <v>147</v>
-      </c>
-      <c r="H23" t="s">
-        <v>75</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="J23" s="8">
-        <v>2.8799999999999999E-2</v>
-      </c>
-      <c r="K23" s="8">
-        <f t="shared" si="0"/>
-        <v>5.7599999999999998E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>226</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D24" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" t="s">
-        <v>240</v>
-      </c>
-      <c r="F24" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" t="s">
-        <v>242</v>
-      </c>
       <c r="H24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>243</v>
+        <v>148</v>
       </c>
       <c r="J24" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="K24" s="8">
         <f t="shared" si="0"/>
+        <v>5.7599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D25" t="s">
+        <v>145</v>
+      </c>
+      <c r="E25" t="s">
+        <v>239</v>
+      </c>
+      <c r="F25" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" t="s">
+        <v>241</v>
+      </c>
+      <c r="H25" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="J25" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
+      <c r="K25" s="8">
+        <f t="shared" si="0"/>
+        <v>2.8799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>2</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D25" t="s">
-        <v>146</v>
-      </c>
-      <c r="E25" t="s">
-        <v>150</v>
-      </c>
-      <c r="F25" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="D26" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" t="s">
+        <v>151</v>
+      </c>
+      <c r="H26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="H25" t="s">
-        <v>75</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="J25" s="8">
+      <c r="J26" s="8">
         <v>2.8400000000000002E-2</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K26" s="8">
         <f t="shared" si="0"/>
         <v>5.6800000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>33</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" t="s">
-        <v>146</v>
-      </c>
-      <c r="E26" t="s">
-        <v>154</v>
-      </c>
-      <c r="F26" t="s">
-        <v>100</v>
-      </c>
-      <c r="G26" t="s">
-        <v>158</v>
-      </c>
-      <c r="H26" t="s">
-        <v>75</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="J26" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="K26" s="8">
-        <f t="shared" si="0"/>
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>228</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>234</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E27" t="s">
-        <v>244</v>
+        <v>153</v>
       </c>
       <c r="F27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G27" t="s">
-        <v>245</v>
+        <v>157</v>
       </c>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>248</v>
+        <v>162</v>
       </c>
       <c r="J27" s="8">
-        <v>3.0200000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="0"/>
-        <v>3.0200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>227</v>
       </c>
@@ -2735,205 +2761,205 @@
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E28" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G28" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>247</v>
       </c>
       <c r="J28" s="8">
-        <v>2.8400000000000002E-2</v>
+        <v>3.0200000000000001E-2</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="0"/>
-        <v>2.8400000000000002E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+        <v>3.0200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>226</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>36</v>
+        <v>234</v>
       </c>
       <c r="D29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E29" t="s">
-        <v>155</v>
+        <v>240</v>
       </c>
       <c r="F29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G29" t="s">
-        <v>164</v>
+        <v>245</v>
       </c>
       <c r="H29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>165</v>
+        <v>246</v>
       </c>
       <c r="J29" s="8">
-        <v>2.86E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K29" s="8">
         <f t="shared" si="0"/>
-        <v>2.86E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+        <v>2.8400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G30" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J30" s="8">
-        <v>0.03</v>
+        <v>2.86E-2</v>
       </c>
       <c r="K30" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+        <v>2.86E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" t="s">
+        <v>158</v>
+      </c>
+      <c r="H31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="K31" s="8">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D31" t="s">
-        <v>146</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D32" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" t="s">
+        <v>166</v>
+      </c>
+      <c r="F32" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" t="s">
         <v>167</v>
       </c>
-      <c r="F31" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="H32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="H31" t="s">
-        <v>75</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="J31" s="8">
+      <c r="J32" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K32" s="8">
         <f t="shared" si="0"/>
         <v>2.8799999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>231</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D32" t="s">
-        <v>146</v>
-      </c>
-      <c r="E32" t="s">
-        <v>275</v>
-      </c>
-      <c r="F32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G32" t="s">
-        <v>276</v>
-      </c>
-      <c r="H32" t="s">
-        <v>75</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="J32" s="8">
-        <v>3.7900000000000003E-2</v>
-      </c>
-      <c r="K32" s="8">
-        <f t="shared" si="0"/>
-        <v>7.5800000000000006E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E33" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G33" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="J33" s="8">
         <v>3.7900000000000003E-2</v>
@@ -2943,282 +2969,282 @@
         <v>7.5800000000000006E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>231</v>
       </c>
       <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D34" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" t="s">
+        <v>277</v>
+      </c>
+      <c r="F34" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" t="s">
+        <v>278</v>
+      </c>
+      <c r="H34" t="s">
+        <v>74</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J34" s="8">
+        <v>3.7900000000000003E-2</v>
+      </c>
+      <c r="K34" s="8">
+        <f t="shared" si="0"/>
+        <v>7.5800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35">
         <v>5</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C35" s="2">
         <v>100</v>
       </c>
-      <c r="D34" t="s">
-        <v>146</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D35" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" t="s">
+        <v>169</v>
+      </c>
+      <c r="F35" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" t="s">
         <v>170</v>
       </c>
-      <c r="F34" t="s">
-        <v>100</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="H35" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="H34" t="s">
-        <v>75</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="J34" s="8">
+      <c r="J35" s="8">
         <v>0.03</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K35" s="8">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>41</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>1</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D35" t="s">
-        <v>146</v>
-      </c>
-      <c r="E35" t="s">
-        <v>157</v>
-      </c>
-      <c r="F35" t="s">
-        <v>100</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="D36" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" t="s">
+        <v>156</v>
+      </c>
+      <c r="F36" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" t="s">
+        <v>159</v>
+      </c>
+      <c r="H36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="J36" s="8">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="K36" s="8">
+        <f t="shared" si="0"/>
+        <v>2.8799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" s="2">
+        <v>470</v>
+      </c>
+      <c r="D37" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" t="s">
+        <v>178</v>
+      </c>
+      <c r="G37" t="s">
+        <v>179</v>
+      </c>
+      <c r="H37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="J37" s="8">
+        <v>7.8600000000000003E-2</v>
+      </c>
+      <c r="K37" s="8">
+        <f t="shared" si="0"/>
+        <v>0.15720000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E38" t="s">
+        <v>181</v>
+      </c>
+      <c r="F38" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" t="s">
         <v>160</v>
       </c>
-      <c r="H35" t="s">
-        <v>75</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="J35" s="8">
-        <v>2.8799999999999999E-2</v>
-      </c>
-      <c r="K35" s="8">
-        <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36" s="2">
-        <v>470</v>
-      </c>
-      <c r="D36" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="H38" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="J38" s="8">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="K38" s="8">
+        <f t="shared" si="0"/>
+        <v>0.11360000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" t="s">
+        <v>145</v>
+      </c>
+      <c r="E39" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" t="s">
+        <v>186</v>
+      </c>
+      <c r="H39" t="s">
+        <v>74</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="J39" s="8">
+        <v>2.8299999999999999E-2</v>
+      </c>
+      <c r="K39" s="8">
+        <f t="shared" si="0"/>
+        <v>0.14149999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>285</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" t="s">
+        <v>145</v>
+      </c>
+      <c r="E40" t="s">
+        <v>182</v>
+      </c>
+      <c r="F40" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" t="s">
+        <v>188</v>
+      </c>
+      <c r="H40" t="s">
+        <v>74</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="J40" s="8">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="K40" s="8">
+        <f t="shared" si="0"/>
+        <v>8.5199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2">
+        <v>560</v>
+      </c>
+      <c r="D41" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" t="s">
         <v>176</v>
       </c>
-      <c r="F36" t="s">
-        <v>179</v>
-      </c>
-      <c r="G36" t="s">
-        <v>180</v>
-      </c>
-      <c r="H36" t="s">
-        <v>75</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="J36" s="8">
-        <v>7.8600000000000003E-2</v>
-      </c>
-      <c r="K36" s="8">
-        <f t="shared" si="0"/>
-        <v>0.15720000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37">
-        <v>4</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" t="s">
-        <v>146</v>
-      </c>
-      <c r="E37" t="s">
-        <v>182</v>
-      </c>
-      <c r="F37" t="s">
-        <v>100</v>
-      </c>
-      <c r="G37" t="s">
-        <v>161</v>
-      </c>
-      <c r="H37" t="s">
-        <v>75</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="J37" s="8">
-        <v>2.8400000000000002E-2</v>
-      </c>
-      <c r="K37" s="8">
-        <f t="shared" si="0"/>
-        <v>0.11360000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" t="s">
-        <v>146</v>
-      </c>
-      <c r="E38" t="s">
-        <v>186</v>
-      </c>
-      <c r="F38" t="s">
-        <v>100</v>
-      </c>
-      <c r="G38" t="s">
-        <v>187</v>
-      </c>
-      <c r="H38" t="s">
-        <v>75</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="J38" s="8">
-        <v>2.8299999999999999E-2</v>
-      </c>
-      <c r="K38" s="8">
-        <f t="shared" si="0"/>
-        <v>0.14149999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" t="s">
-        <v>146</v>
-      </c>
-      <c r="E39" t="s">
-        <v>183</v>
-      </c>
-      <c r="F39" t="s">
-        <v>100</v>
-      </c>
-      <c r="G39" t="s">
-        <v>189</v>
-      </c>
-      <c r="H39" t="s">
-        <v>75</v>
-      </c>
-      <c r="I39" s="7" t="s">
+      <c r="F41" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41" t="s">
         <v>190</v>
       </c>
-      <c r="J39" s="8">
-        <v>2.8400000000000002E-2</v>
-      </c>
-      <c r="K39" s="8">
-        <f t="shared" si="0"/>
-        <v>0.11360000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" s="2">
-        <v>560</v>
-      </c>
-      <c r="D40" t="s">
-        <v>146</v>
-      </c>
-      <c r="E40" t="s">
-        <v>177</v>
-      </c>
-      <c r="F40" t="s">
-        <v>100</v>
-      </c>
-      <c r="G40" t="s">
-        <v>191</v>
-      </c>
-      <c r="H40" t="s">
-        <v>75</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="J40" s="8">
-        <v>2.8799999999999999E-2</v>
-      </c>
-      <c r="K40" s="8">
-        <f t="shared" si="0"/>
-        <v>2.8799999999999999E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>193</v>
-      </c>
-      <c r="B41">
-        <v>11</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" t="s">
-        <v>184</v>
-      </c>
-      <c r="F41" t="s">
-        <v>100</v>
-      </c>
-      <c r="G41" t="s">
-        <v>162</v>
-      </c>
       <c r="H41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>194</v>
@@ -3228,304 +3254,340 @@
       </c>
       <c r="K41" s="8">
         <f t="shared" si="0"/>
-        <v>0.31679999999999997</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+        <v>2.8799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>192</v>
       </c>
       <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E42" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="F42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G42" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="H42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
       <c r="J42" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="K42" s="8">
         <f t="shared" si="0"/>
+        <v>0.31679999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>145</v>
+      </c>
+      <c r="E43" t="s">
+        <v>177</v>
+      </c>
+      <c r="F43" t="s">
+        <v>99</v>
+      </c>
+      <c r="G43" t="s">
+        <v>147</v>
+      </c>
+      <c r="H43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="J43" s="8">
         <v>2.8799999999999999E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D43" t="s">
-        <v>197</v>
-      </c>
-      <c r="E43" t="s">
-        <v>199</v>
-      </c>
-      <c r="F43" t="s">
-        <v>200</v>
-      </c>
-      <c r="G43" t="s">
-        <v>201</v>
-      </c>
-      <c r="H43" t="s">
-        <v>114</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="J43" s="8">
-        <v>1.5</v>
-      </c>
       <c r="K43" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+        <v>2.8799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>174</v>
+        <v>52</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D44" t="s">
+        <v>196</v>
+      </c>
+      <c r="E44" t="s">
+        <v>198</v>
+      </c>
+      <c r="F44" t="s">
+        <v>199</v>
+      </c>
+      <c r="G44" t="s">
+        <v>200</v>
+      </c>
+      <c r="H44" t="s">
+        <v>113</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="J44" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="K44" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" s="2">
         <v>100</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" t="s">
         <v>206</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F45" t="s">
+        <v>72</v>
+      </c>
+      <c r="G45" t="s">
         <v>207</v>
       </c>
-      <c r="F44" t="s">
-        <v>73</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="H45" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="H44" t="s">
-        <v>75</v>
-      </c>
-      <c r="I44" s="7" t="s">
+      <c r="J45" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="K45" s="8">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" t="s">
+        <v>197</v>
+      </c>
+      <c r="E46" t="s">
+        <v>202</v>
+      </c>
+      <c r="F46" t="s">
+        <v>199</v>
+      </c>
+      <c r="G46" t="s">
+        <v>203</v>
+      </c>
+      <c r="H46" t="s">
+        <v>113</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="J46" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="K46" s="8">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" t="s">
         <v>209</v>
       </c>
-      <c r="J44" s="8">
-        <v>1.4</v>
-      </c>
-      <c r="K44" s="8">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>192</v>
-      </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D45" t="s">
-        <v>198</v>
-      </c>
-      <c r="E45" t="s">
-        <v>203</v>
-      </c>
-      <c r="F45" t="s">
-        <v>200</v>
-      </c>
-      <c r="G45" t="s">
-        <v>204</v>
-      </c>
-      <c r="H45" t="s">
-        <v>114</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="J45" s="8">
-        <v>1.25</v>
-      </c>
-      <c r="K45" s="8">
-        <f t="shared" si="0"/>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46">
-        <v>6</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="E47" t="s">
+        <v>210</v>
+      </c>
+      <c r="F47" t="s">
+        <v>211</v>
+      </c>
+      <c r="G47" t="s">
+        <v>212</v>
+      </c>
+      <c r="H47" t="s">
+        <v>74</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="J47" s="8">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="K47" s="8">
+        <f t="shared" si="0"/>
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>56</v>
-      </c>
-      <c r="D46" t="s">
-        <v>210</v>
-      </c>
-      <c r="E46" t="s">
-        <v>211</v>
-      </c>
-      <c r="F46" t="s">
-        <v>212</v>
-      </c>
-      <c r="G46" t="s">
-        <v>213</v>
-      </c>
-      <c r="H46" t="s">
-        <v>75</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="J46" s="8">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="K46" s="8">
-        <f t="shared" si="0"/>
-        <v>5.43</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" t="s">
-        <v>215</v>
-      </c>
-      <c r="E47" t="s">
-        <v>216</v>
-      </c>
-      <c r="F47" t="s">
-        <v>212</v>
-      </c>
-      <c r="G47" t="s">
-        <v>217</v>
-      </c>
-      <c r="H47" t="s">
-        <v>75</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="J47" s="8">
-        <v>1.84</v>
-      </c>
-      <c r="K47" s="8">
-        <f t="shared" si="0"/>
-        <v>1.84</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>59</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D48" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E48" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F48" t="s">
-        <v>109</v>
+        <v>211</v>
       </c>
       <c r="G48" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J48" s="8">
-        <v>0.46</v>
+        <v>1.84</v>
       </c>
       <c r="K48" s="8">
         <f t="shared" si="0"/>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D49" t="s">
+        <v>218</v>
+      </c>
+      <c r="E49" t="s">
         <v>219</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
+        <v>108</v>
+      </c>
+      <c r="G49" t="s">
+        <v>220</v>
+      </c>
+      <c r="H49" t="s">
+        <v>74</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="J49" s="8">
+        <v>0.46</v>
+      </c>
+      <c r="K49" s="8">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" t="s">
+        <v>218</v>
+      </c>
+      <c r="E50" t="s">
+        <v>222</v>
+      </c>
+      <c r="F50" t="s">
+        <v>108</v>
+      </c>
+      <c r="G50" t="s">
         <v>223</v>
       </c>
-      <c r="F49" t="s">
-        <v>109</v>
-      </c>
-      <c r="G49" t="s">
+      <c r="H50" t="s">
+        <v>113</v>
+      </c>
+      <c r="I50" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="H49" t="s">
-        <v>114</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="J49" s="8">
+      <c r="J50" s="8">
         <v>0.40400000000000003</v>
       </c>
-      <c r="K49" s="8">
+      <c r="K50" s="8">
         <f t="shared" si="0"/>
         <v>0.40400000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J51" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="K51" s="4">
-        <f>SUM(K2:K49)</f>
-        <v>29.3781</v>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J52" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K52" s="4">
+        <f>SUM(K2:K50)</f>
+        <v>29.3704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>